<commit_message>
Added Data Cleaning code
</commit_message>
<xml_diff>
--- a/Financial_Data/MoneyControl/Companies/IT Services & Consulting/3i Infotech Ltd/Excel/Cash-flow_combined.xlsx
+++ b/Financial_Data/MoneyControl/Companies/IT Services & Consulting/3i Infotech Ltd/Excel/Cash-flow_combined.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sharm\OneDrive\Desktop\Kishan\Contractzy\WebScrapping\Tutorial\Financial_Data\MoneyControl\Companies\IT Services &amp; Consulting\3i Infotech Ltd\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D23B6AF-AE36-4548-AA2A-3D996C3CE990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCBCA6D4-D9C1-4788-8CFC-6E460294F211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="157">
   <si>
     <t>Cash Flow of 3i Infotech(in Rs. Cr.)</t>
   </si>
@@ -491,12 +491,6 @@
   </si>
   <si>
     <t>67.24</t>
-  </si>
-  <si>
-    <t>str</t>
-  </si>
-  <si>
-    <t>nan</t>
   </si>
 </sst>
 </file>
@@ -864,10 +858,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U16"/>
+  <dimension ref="A1:U11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1588,19 +1582,6 @@
         <v>156</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="C16" t="s">
-        <v>157</v>
-      </c>
-      <c r="D16" t="s">
-        <v>157</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>